<commit_message>
fixing up example, adding submodule design
</commit_message>
<xml_diff>
--- a/example/points.xlsx
+++ b/example/points.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
-  <si>
-    <t xml:space="preserve">ref des</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">source ref des</t>
   </si>
   <si>
     <t xml:space="preserve">test point ref des</t>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">TP6</t>
   </si>
   <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP7</t>
   </si>
   <si>
@@ -76,15 +79,15 @@
     <t xml:space="preserve">TP14</t>
   </si>
   <si>
-    <t xml:space="preserve">J4</t>
-  </si>
-  <si>
     <t xml:space="preserve">TP15</t>
   </si>
   <si>
     <t xml:space="preserve">TP16</t>
   </si>
   <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP17</t>
   </si>
   <si>
@@ -95,33 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">TP20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP27</t>
   </si>
 </sst>
 </file>
@@ -224,11 +200,11 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -333,7 +309,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
@@ -344,288 +320,232 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>8</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>9</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>